<commit_message>
Major fixes, new analyses, new data
</commit_message>
<xml_diff>
--- a/data/spreadsheets/data.xlsx
+++ b/data/spreadsheets/data.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,17 +457,22 @@
     <row r="1">
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\thead{Clustering\\Coefficient}</t>
+          <t>Clustering Coefficient</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>\thead{Edge\\Distance}</t>
+          <t>Edge Distance</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>\thead{Total\\Bidirectional\\Links}</t>
+          <t>Total Bidirectional Links</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Average Connectivity</t>
         </is>
       </c>
     </row>
@@ -483,13 +488,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.03630741610516294</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>17.59380225153841</v>
+        <v>16.27</v>
       </c>
       <c r="E2" t="n">
-        <v>11.169</v>
+        <v>22.77</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.86</v>
       </c>
     </row>
     <row r="3">
@@ -500,13 +508,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1362189162132003</v>
+        <v>0.14</v>
       </c>
       <c r="D3" t="n">
-        <v>6.6078085836607</v>
+        <v>6.62</v>
       </c>
       <c r="E3" t="n">
-        <v>82.84099999999999</v>
+        <v>82.41</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="4">
@@ -517,108 +528,166 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.02858906973237614</v>
+        <v>0.03</v>
       </c>
       <c r="D4" t="n">
-        <v>19.15215193568061</v>
+        <v>19.07</v>
       </c>
       <c r="E4" t="n">
-        <v>6.943</v>
+        <v>7.23</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
+          <t>REEM</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D5" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>33.92</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
           <t>CENN</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0.1157792471279743</v>
-      </c>
-      <c r="D5" t="n">
-        <v>15.32748866218518</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="C6" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D6" t="n">
+        <v>15.33</v>
+      </c>
+      <c r="E6" t="n">
         <v>50</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="F6" t="n">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Adult</t>
         </is>
       </c>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>SEEM</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0.09088266609755791</v>
-      </c>
-      <c r="D6" t="n">
-        <v>17.58911342699803</v>
-      </c>
-      <c r="E6" t="n">
-        <v>68.313</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="inlineStr">
-        <is>
-          <t>RDDA</t>
-        </is>
-      </c>
       <c r="C7" t="n">
-        <v>0.2534091269676462</v>
+        <v>0.17</v>
       </c>
       <c r="D7" t="n">
-        <v>7.550170793661431</v>
+        <v>16.27</v>
       </c>
       <c r="E7" t="n">
-        <v>284.917</v>
+        <v>116.52</v>
+      </c>
+      <c r="F7" t="n">
+        <v>15.05</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>ERN</t>
+          <t>RDDA</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.07052296465055713</v>
+        <v>0.24</v>
       </c>
       <c r="D8" t="n">
-        <v>19.19376111274872</v>
+        <v>7.39</v>
       </c>
       <c r="E8" t="n">
-        <v>42.652</v>
+        <v>251.76</v>
+      </c>
+      <c r="F8" t="n">
+        <v>18.38</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
       <c r="B9" s="1" t="inlineStr">
         <is>
+          <t>ERN</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D9" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>35.13</v>
+      </c>
+      <c r="F9" t="n">
+        <v>20.23</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="1" t="inlineStr">
+        <is>
+          <t>REEM</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="D10" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E10" t="n">
+        <v>175.25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>18.09</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
           <t>CENN</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>0.1973186976274788</v>
-      </c>
-      <c r="D9" t="n">
-        <v>15.17037411643299</v>
-      </c>
-      <c r="E9" t="n">
-        <v>150.3333333333333</v>
+      <c r="C11" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15.17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>150.33</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4.6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A2:A6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data for bidirectional electrical synapses
</commit_message>
<xml_diff>
--- a/data/spreadsheets/data.xlsx
+++ b/data/spreadsheets/data.xlsx
@@ -488,16 +488,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="D2" t="n">
-        <v>16.27</v>
+        <v>16.23</v>
       </c>
       <c r="E2" t="n">
-        <v>22.77</v>
+        <v>26.62</v>
       </c>
       <c r="F2" t="n">
-        <v>1.86</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="3">
@@ -508,16 +508,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="D3" t="n">
-        <v>6.62</v>
+        <v>6.69</v>
       </c>
       <c r="E3" t="n">
-        <v>82.41</v>
+        <v>94.81</v>
       </c>
       <c r="F3" t="n">
-        <v>2.24</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="4">
@@ -531,13 +531,13 @@
         <v>0.03</v>
       </c>
       <c r="D4" t="n">
-        <v>19.07</v>
+        <v>19.17</v>
       </c>
       <c r="E4" t="n">
-        <v>7.23</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>2.59</v>
+        <v>2.89</v>
       </c>
     </row>
     <row r="5">
@@ -548,16 +548,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>17.1</v>
+        <v>16.36</v>
       </c>
       <c r="E5" t="n">
-        <v>33.92</v>
+        <v>44.44</v>
       </c>
       <c r="F5" t="n">
-        <v>2.33</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="6">
@@ -571,13 +571,13 @@
         <v>0.12</v>
       </c>
       <c r="D6" t="n">
-        <v>15.33</v>
+        <v>15.11</v>
       </c>
       <c r="E6" t="n">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="F6" t="n">
-        <v>1.35</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="7">
@@ -592,16 +592,16 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="D7" t="n">
-        <v>16.27</v>
+        <v>16.25</v>
       </c>
       <c r="E7" t="n">
-        <v>116.52</v>
+        <v>146.76</v>
       </c>
       <c r="F7" t="n">
-        <v>15.05</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -612,16 +612,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="D8" t="n">
-        <v>7.39</v>
+        <v>7.58</v>
       </c>
       <c r="E8" t="n">
-        <v>251.76</v>
+        <v>288.59</v>
       </c>
       <c r="F8" t="n">
-        <v>18.46</v>
+        <v>20.98</v>
       </c>
     </row>
     <row r="9">
@@ -632,16 +632,16 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.06</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D9" t="n">
         <v>19.2</v>
       </c>
       <c r="E9" t="n">
-        <v>35.13</v>
+        <v>44.84</v>
       </c>
       <c r="F9" t="n">
-        <v>20.23</v>
+        <v>23.08</v>
       </c>
     </row>
     <row r="10">
@@ -652,16 +652,16 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.14</v>
+        <v>0.16</v>
       </c>
       <c r="D10" t="n">
-        <v>16.86</v>
+        <v>16.38</v>
       </c>
       <c r="E10" t="n">
-        <v>178.16</v>
+        <v>236.49</v>
       </c>
       <c r="F10" t="n">
-        <v>18.02</v>
+        <v>20.27</v>
       </c>
     </row>
     <row r="11">
@@ -672,16 +672,16 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="D11" t="n">
-        <v>15.17</v>
+        <v>14.94</v>
       </c>
       <c r="E11" t="n">
-        <v>150.33</v>
+        <v>283.33</v>
       </c>
       <c r="F11" t="n">
-        <v>4.6</v>
+        <v>5.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>